<commit_message>
add a couple of more pages
</commit_message>
<xml_diff>
--- a/data/the_one_we_need.xlsx
+++ b/data/the_one_we_need.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusiyao/Desktop/VT/STAT_4664_Stochastic/final/data/anopheles_gambiae/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusiyao/Desktop/VT/STAT_4664_Stochastic/final/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E56DD54-1F0E-A24B-B746-E40E93DAEF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F82D623-9F14-314B-A246-DEEC99AF8EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="27640" windowHeight="16880" xr2:uid="{5C172BC8-147F-7C4A-A66B-921FD0C4B46E}"/>
+    <workbookView xWindow="1060" yWindow="1680" windowWidth="23440" windowHeight="17280" xr2:uid="{5C172BC8-147F-7C4A-A66B-921FD0C4B46E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="90">
   <si>
     <t>Id</t>
   </si>
@@ -677,13 +677,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0C8862-E0E3-BF47-BB41-CEE184F341FB}">
-  <dimension ref="A1:AX11"/>
+  <dimension ref="A1:AX9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="39.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="15" max="15" width="45.6640625" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="21.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -839,7 +851,7 @@
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>88353</v>
+        <v>88354</v>
       </c>
       <c r="B2">
         <v>436</v>
@@ -854,13 +866,13 @@
         <v>52</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
         <v>53</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2" t="s">
         <v>54</v>
@@ -899,7 +911,7 @@
         <v>62</v>
       </c>
       <c r="U2">
-        <v>92</v>
+        <v>273</v>
       </c>
       <c r="V2" t="s">
         <v>63</v>
@@ -929,7 +941,7 @@
         <v>71</v>
       </c>
       <c r="AE2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AF2" t="s">
         <v>58</v>
@@ -991,7 +1003,7 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>88354</v>
+        <v>88355</v>
       </c>
       <c r="B3">
         <v>436</v>
@@ -1006,13 +1018,13 @@
         <v>52</v>
       </c>
       <c r="F3">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
         <v>53</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" t="s">
         <v>54</v>
@@ -1051,7 +1063,7 @@
         <v>62</v>
       </c>
       <c r="U3">
-        <v>273</v>
+        <v>322</v>
       </c>
       <c r="V3" t="s">
         <v>63</v>
@@ -1081,7 +1093,7 @@
         <v>71</v>
       </c>
       <c r="AE3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AF3" t="s">
         <v>58</v>
@@ -1132,7 +1144,7 @@
         <v>84</v>
       </c>
       <c r="AV3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AW3" t="s">
         <v>30</v>
@@ -1143,7 +1155,7 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>88355</v>
+        <v>88356</v>
       </c>
       <c r="B4">
         <v>436</v>
@@ -1158,13 +1170,13 @@
         <v>52</v>
       </c>
       <c r="F4">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
         <v>53</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
         <v>54</v>
@@ -1203,7 +1215,7 @@
         <v>62</v>
       </c>
       <c r="U4">
-        <v>322</v>
+        <v>114</v>
       </c>
       <c r="V4" t="s">
         <v>63</v>
@@ -1233,7 +1245,7 @@
         <v>71</v>
       </c>
       <c r="AE4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AF4" t="s">
         <v>58</v>
@@ -1295,7 +1307,7 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>88356</v>
+        <v>88358</v>
       </c>
       <c r="B5">
         <v>436</v>
@@ -1310,13 +1322,13 @@
         <v>52</v>
       </c>
       <c r="F5">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
         <v>53</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
         <v>54</v>
@@ -1331,7 +1343,7 @@
         <v>57</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N5" t="s">
         <v>58</v>
@@ -1355,7 +1367,7 @@
         <v>62</v>
       </c>
       <c r="U5">
-        <v>114</v>
+        <v>377</v>
       </c>
       <c r="V5" t="s">
         <v>63</v>
@@ -1385,7 +1397,7 @@
         <v>71</v>
       </c>
       <c r="AE5">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AF5" t="s">
         <v>58</v>
@@ -1436,7 +1448,7 @@
         <v>84</v>
       </c>
       <c r="AV5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AW5" t="s">
         <v>30</v>
@@ -1447,7 +1459,7 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>88357</v>
+        <v>88359</v>
       </c>
       <c r="B6">
         <v>436</v>
@@ -1462,13 +1474,13 @@
         <v>52</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
         <v>53</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6" t="s">
         <v>54</v>
@@ -1507,7 +1519,7 @@
         <v>62</v>
       </c>
       <c r="U6">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="V6" t="s">
         <v>63</v>
@@ -1537,7 +1549,7 @@
         <v>71</v>
       </c>
       <c r="AE6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="AF6" t="s">
         <v>58</v>
@@ -1599,10 +1611,10 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>88358</v>
+        <v>88360</v>
       </c>
       <c r="B7">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C7" t="s">
         <v>50</v>
@@ -1614,13 +1626,13 @@
         <v>52</v>
       </c>
       <c r="F7">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I7" t="s">
         <v>54</v>
@@ -1635,7 +1647,7 @@
         <v>57</v>
       </c>
       <c r="M7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N7" t="s">
         <v>58</v>
@@ -1656,10 +1668,10 @@
         <v>-77.054028000000002</v>
       </c>
       <c r="T7" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="U7">
-        <v>377</v>
+        <v>273</v>
       </c>
       <c r="V7" t="s">
         <v>63</v>
@@ -1680,7 +1692,7 @@
         <v>68</v>
       </c>
       <c r="AB7" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="AC7" t="s">
         <v>70</v>
@@ -1689,7 +1701,7 @@
         <v>71</v>
       </c>
       <c r="AE7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AF7" t="s">
         <v>58</v>
@@ -1740,7 +1752,7 @@
         <v>84</v>
       </c>
       <c r="AV7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AW7" t="s">
         <v>30</v>
@@ -1751,10 +1763,10 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>88359</v>
+        <v>88361</v>
       </c>
       <c r="B8">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C8" t="s">
         <v>50</v>
@@ -1766,7 +1778,7 @@
         <v>52</v>
       </c>
       <c r="F8">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
@@ -1787,7 +1799,7 @@
         <v>57</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N8" t="s">
         <v>58</v>
@@ -1808,10 +1820,10 @@
         <v>-77.054028000000002</v>
       </c>
       <c r="T8" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="U8">
-        <v>228</v>
+        <v>383</v>
       </c>
       <c r="V8" t="s">
         <v>63</v>
@@ -1832,7 +1844,7 @@
         <v>68</v>
       </c>
       <c r="AB8" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="AC8" t="s">
         <v>70</v>
@@ -1841,7 +1853,7 @@
         <v>71</v>
       </c>
       <c r="AE8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AF8" t="s">
         <v>58</v>
@@ -1892,7 +1904,7 @@
         <v>84</v>
       </c>
       <c r="AV8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AW8" t="s">
         <v>30</v>
@@ -1903,7 +1915,7 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>88360</v>
+        <v>88362</v>
       </c>
       <c r="B9">
         <v>437</v>
@@ -1918,7 +1930,7 @@
         <v>52</v>
       </c>
       <c r="F9">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
         <v>53</v>
@@ -1939,7 +1951,7 @@
         <v>57</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N9" t="s">
         <v>58</v>
@@ -1963,7 +1975,7 @@
         <v>88</v>
       </c>
       <c r="U9">
-        <v>273</v>
+        <v>491</v>
       </c>
       <c r="V9" t="s">
         <v>63</v>
@@ -1993,7 +2005,7 @@
         <v>71</v>
       </c>
       <c r="AE9">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AF9" t="s">
         <v>58</v>
@@ -2044,316 +2056,12 @@
         <v>84</v>
       </c>
       <c r="AV9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AW9" t="s">
         <v>30</v>
       </c>
       <c r="AX9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>88361</v>
-      </c>
-      <c r="B10">
-        <v>437</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J10" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>58</v>
-      </c>
-      <c r="O10" t="s">
-        <v>59</v>
-      </c>
-      <c r="P10" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>61</v>
-      </c>
-      <c r="R10">
-        <v>39.005000000000003</v>
-      </c>
-      <c r="S10">
-        <v>-77.054028000000002</v>
-      </c>
-      <c r="T10" t="s">
-        <v>88</v>
-      </c>
-      <c r="U10">
-        <v>383</v>
-      </c>
-      <c r="V10" t="s">
-        <v>63</v>
-      </c>
-      <c r="W10" t="s">
-        <v>64</v>
-      </c>
-      <c r="X10" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE10">
-        <v>19</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG10">
-        <v>27</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>74</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>75</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>76</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>78</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ10" t="s">
-        <v>80</v>
-      </c>
-      <c r="AR10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AS10" t="s">
-        <v>82</v>
-      </c>
-      <c r="AT10" t="s">
-        <v>83</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AV10" t="s">
-        <v>86</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>30</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>88362</v>
-      </c>
-      <c r="B11">
-        <v>437</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="I11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11">
-        <v>5</v>
-      </c>
-      <c r="N11" t="s">
-        <v>58</v>
-      </c>
-      <c r="O11" t="s">
-        <v>59</v>
-      </c>
-      <c r="P11" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R11">
-        <v>39.005000000000003</v>
-      </c>
-      <c r="S11">
-        <v>-77.054028000000002</v>
-      </c>
-      <c r="T11" t="s">
-        <v>88</v>
-      </c>
-      <c r="U11">
-        <v>491</v>
-      </c>
-      <c r="V11" t="s">
-        <v>63</v>
-      </c>
-      <c r="W11" t="s">
-        <v>64</v>
-      </c>
-      <c r="X11" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE11">
-        <v>19</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG11">
-        <v>27</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>74</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>76</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AP11" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AR11" t="s">
-        <v>81</v>
-      </c>
-      <c r="AS11" t="s">
-        <v>82</v>
-      </c>
-      <c r="AT11" t="s">
-        <v>83</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AV11" t="s">
-        <v>87</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>30</v>
-      </c>
-      <c r="AX11" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>